<commit_message>
P14 completado com sucesso para STM32F407.
</commit_message>
<xml_diff>
--- a/STM32F407/STM32F407ZG_BlackBoard_Pinout.xlsx
+++ b/STM32F407/STM32F407ZG_BlackBoard_Pinout.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19155" windowHeight="6465" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19155" windowHeight="6465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
     <sheet name="MCU" sheetId="2" r:id="rId2"/>
     <sheet name="SPI" sheetId="3" r:id="rId3"/>
     <sheet name="ADC" sheetId="4" r:id="rId4"/>
+    <sheet name="I2C" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MCU!$A$1:$Q$145</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="443">
   <si>
     <t>J2</t>
   </si>
@@ -1377,6 +1378,9 @@
   </si>
   <si>
     <t>Descrição</t>
+  </si>
+  <si>
+    <t>I2C #</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1495,6 +1499,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -2520,7 +2525,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4086,7 +4091,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4981,9 +4986,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q145">
-    <filterColumn colId="1">
+    <filterColumn colId="7">
       <filters>
-        <filter val="PC15-OSC32_OUT"/>
+        <filter val="I2C3_SDA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4996,7 +5001,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,7 +5333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="14" t="s">
         <v>416</v>
@@ -5351,7 +5356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -5658,4 +5663,204 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="2">
+        <v>136</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="9">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="2">
+        <v>137</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="9">
+        <v>140</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="9">
+        <v>69</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="9">
+        <v>70</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="2">
+        <v>99</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>